<commit_message>
removed original xl-2-pan files
</commit_message>
<xml_diff>
--- a/tools/xl-2-pan/xl-tmplt.xlsx
+++ b/tools/xl-2-pan/xl-tmplt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcameron/Repositories/T3Net-Automation/tools/xl-2-pan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F23390-9A28-6A4C-BD94-4B3C75BC400B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4B3A17-EA5D-9949-9874-0CF7DDC4F67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-77060" yWindow="4160" windowWidth="32420" windowHeight="27820" activeTab="1" xr2:uid="{1ED8597C-C799-1844-91B8-6CEA0FE6763F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="240">
   <si>
     <t>Vlan_903</t>
   </si>
@@ -4943,7 +4943,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH3" sqref="AH3"/>
+      <selection pane="bottomLeft" activeCell="AK31" sqref="AK31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -5220,14 +5220,17 @@
       <c r="AG3" s="2" t="s">
         <v>228</v>
       </c>
+      <c r="AH3" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="AI3" s="1" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="AJ3" s="1" t="s">
         <v>187</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="AL3" s="2" t="s">
         <v>180</v>

</xml_diff>